<commit_message>
Almost there (last review missing)
</commit_message>
<xml_diff>
--- a/database_akasha.xlsx
+++ b/database_akasha.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Desktop\MasterThesis\GHG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32823243-610A-41F4-995C-06CBDB98E8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1223775-6BBD-422C-9E0A-F5B31F56CB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-6015" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PROJECT_PHASES" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="93">
   <si>
     <t>project_phase</t>
   </si>
@@ -131,9 +131,6 @@
     <t>m2</t>
   </si>
   <si>
-    <t>ton CO2eq / year</t>
-  </si>
-  <si>
     <t>stream</t>
   </si>
   <si>
@@ -203,122 +200,134 @@
     <t>CONSUMED</t>
   </si>
   <si>
+    <t>Construction Trucks</t>
+  </si>
+  <si>
+    <t>Personnel Transport</t>
+  </si>
+  <si>
+    <t>Material Transport</t>
+  </si>
+  <si>
+    <t>Soil Excavation Trucks</t>
+  </si>
+  <si>
+    <t>Reservoir Liner Trucks</t>
+  </si>
+  <si>
+    <t>General Utility Vehicles</t>
+  </si>
+  <si>
+    <t>ROAD</t>
+  </si>
+  <si>
+    <t>Site Generators</t>
+  </si>
+  <si>
+    <t>Workshop Generator</t>
+  </si>
+  <si>
+    <t>Desalination Backup</t>
+  </si>
+  <si>
+    <t>Excavators</t>
+  </si>
+  <si>
+    <t>Cranes</t>
+  </si>
+  <si>
+    <t>Concrete Mixers</t>
+  </si>
+  <si>
+    <t>Bulldozers</t>
+  </si>
+  <si>
+    <t>Tippers</t>
+  </si>
+  <si>
+    <t>Water Trucks</t>
+  </si>
+  <si>
+    <t>Concrete</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>HDPE Geomembrane</t>
+  </si>
+  <si>
+    <t>Asphalt</t>
+  </si>
+  <si>
+    <t>Gravel</t>
+  </si>
+  <si>
+    <t>Reinforced Bar</t>
+  </si>
+  <si>
+    <t>Water Pumps Backup</t>
+  </si>
+  <si>
+    <t>upper reservoir</t>
+  </si>
+  <si>
+    <t>lower reservoire</t>
+  </si>
+  <si>
+    <t>dam</t>
+  </si>
+  <si>
+    <t>support station</t>
+  </si>
+  <si>
+    <t>desalination station</t>
+  </si>
+  <si>
+    <t>access roads</t>
+  </si>
+  <si>
+    <t>eletric grid</t>
+  </si>
+  <si>
+    <t>pipelines</t>
+  </si>
+  <si>
+    <t>reservoire</t>
+  </si>
+  <si>
+    <t>grassland</t>
+  </si>
+  <si>
+    <t>shrubland</t>
+  </si>
+  <si>
+    <t>sparse vegetation</t>
+  </si>
+  <si>
+    <t>station</t>
+  </si>
+  <si>
+    <t>roads</t>
+  </si>
+  <si>
+    <t>ton CO2eq / m2 / year</t>
+  </si>
+  <si>
+    <t>ton CO2eq / km</t>
+  </si>
+  <si>
     <t>Hydropower Energy Generation</t>
   </si>
   <si>
     <t>PRODUCED</t>
-  </si>
-  <si>
-    <t>Construction Trucks</t>
-  </si>
-  <si>
-    <t>Personnel Transport</t>
-  </si>
-  <si>
-    <t>Material Transport</t>
-  </si>
-  <si>
-    <t>Soil Excavation Trucks</t>
-  </si>
-  <si>
-    <t>Reservoir Liner Trucks</t>
-  </si>
-  <si>
-    <t>General Utility Vehicles</t>
-  </si>
-  <si>
-    <t>ROAD</t>
-  </si>
-  <si>
-    <t>Site Generators</t>
-  </si>
-  <si>
-    <t>Workshop Generator</t>
-  </si>
-  <si>
-    <t>Desalination Backup</t>
-  </si>
-  <si>
-    <t>Excavators</t>
-  </si>
-  <si>
-    <t>Cranes</t>
-  </si>
-  <si>
-    <t>Concrete Mixers</t>
-  </si>
-  <si>
-    <t>Bulldozers</t>
-  </si>
-  <si>
-    <t>Tippers</t>
-  </si>
-  <si>
-    <t>Water Trucks</t>
-  </si>
-  <si>
-    <t>Concrete</t>
-  </si>
-  <si>
-    <t>Steel</t>
-  </si>
-  <si>
-    <t>HDPE Geomembrane</t>
-  </si>
-  <si>
-    <t>Asphalt</t>
-  </si>
-  <si>
-    <t>Gravel</t>
-  </si>
-  <si>
-    <t>Reinforced Bar</t>
-  </si>
-  <si>
-    <t>Excavated Earth</t>
-  </si>
-  <si>
-    <t>Cut Basalt</t>
-  </si>
-  <si>
-    <t>Construction Debris</t>
-  </si>
-  <si>
-    <t>Concrete Waste</t>
-  </si>
-  <si>
-    <t>Steel Scrap</t>
-  </si>
-  <si>
-    <t>Liner Scraps</t>
-  </si>
-  <si>
-    <t>reservoir and tunnel excavation</t>
-  </si>
-  <si>
-    <t>reservoir shaping yields basalt fragments used/reused on site</t>
-  </si>
-  <si>
-    <t>non-hazardous waste from temporary structures</t>
-  </si>
-  <si>
-    <t>HDPE offcuts during geomembrane laying process</t>
-  </si>
-  <si>
-    <t>off-cuts and rebar trimmings during fabrication phase</t>
-  </si>
-  <si>
-    <t>estimated at 3–5% of total concrete volume used</t>
-  </si>
-  <si>
-    <t>Water Pumps Backup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -349,6 +358,19 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -431,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -458,6 +480,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -750,7 +778,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -767,7 +795,7 @@
     </row>
     <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
@@ -776,7 +804,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>9</v>
@@ -784,13 +812,13 @@
     </row>
     <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="6">
         <v>0.5</v>
@@ -801,13 +829,13 @@
     </row>
     <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="6">
         <v>22</v>
@@ -818,13 +846,13 @@
     </row>
     <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="6">
         <v>0.3</v>
@@ -835,16 +863,16 @@
     </row>
     <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="D6" s="6">
-        <v>2325.354166666667</v>
+        <v>2325.3541666666702</v>
       </c>
       <c r="E6" s="6">
         <v>4.0000000000000001E-3</v>
@@ -1193,9 +1221,9 @@
   </sheetPr>
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1216,7 +1244,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1248,7 +1276,7 @@
     </row>
     <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
@@ -1257,36 +1285,36 @@
         <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D3" s="7">
         <v>15000</v>
@@ -1298,13 +1326,13 @@
         <v>1.5E-3</v>
       </c>
       <c r="G3" s="7">
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="H3" s="8">
         <v>25</v>
       </c>
       <c r="I3" s="6">
-        <v>2.0000000000000002E-5</v>
+        <v>0</v>
       </c>
       <c r="J3" s="8">
         <v>298</v>
@@ -1312,13 +1340,13 @@
     </row>
     <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D4" s="7">
         <v>8000</v>
@@ -1330,14 +1358,14 @@
         <v>1.5E-3</v>
       </c>
       <c r="G4" s="7">
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" ref="H4:H51" si="0">IF(ISBLANK(G4), "", $H$3)</f>
         <v>25</v>
       </c>
       <c r="I4" s="7">
-        <v>2.0000000000000002E-5</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" ref="J4:J11" si="1">IF(ISBLANK(I4), "", $J$3)</f>
@@ -1346,13 +1374,13 @@
     </row>
     <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D5" s="7">
         <v>12000</v>
@@ -1364,14 +1392,14 @@
         <v>1.5E-3</v>
       </c>
       <c r="G5" s="7">
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="I5" s="7">
-        <v>2.0000000000000002E-5</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="1"/>
@@ -1380,13 +1408,13 @@
     </row>
     <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D6" s="7">
         <v>10000</v>
@@ -1398,14 +1426,14 @@
         <v>1.5E-3</v>
       </c>
       <c r="G6" s="7">
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="I6" s="7">
-        <v>2.0000000000000002E-5</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="1"/>
@@ -1414,13 +1442,13 @@
     </row>
     <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" s="7">
         <v>7000</v>
@@ -1432,14 +1460,14 @@
         <v>1.5E-3</v>
       </c>
       <c r="G7" s="7">
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="I7" s="7">
-        <v>2.0000000000000002E-5</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="1"/>
@@ -1448,13 +1476,13 @@
     </row>
     <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D8" s="7">
         <v>9000</v>
@@ -1466,14 +1494,14 @@
         <v>1.5E-3</v>
       </c>
       <c r="G8" s="7">
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="I8" s="7">
-        <v>2.0000000000000002E-5</v>
+        <v>0</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="1"/>
@@ -2310,7 +2338,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2327,24 +2355,24 @@
     </row>
     <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>2</v>
@@ -2361,7 +2389,7 @@
     </row>
     <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>3</v>
@@ -2378,7 +2406,7 @@
     </row>
     <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
@@ -2395,7 +2423,7 @@
     </row>
     <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>3</v>
@@ -2753,7 +2781,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2771,7 +2799,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2800,36 +2828,36 @@
     </row>
     <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>2</v>
@@ -2858,7 +2886,7 @@
     </row>
     <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
@@ -2889,7 +2917,7 @@
     </row>
     <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
@@ -2920,7 +2948,7 @@
     </row>
     <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>2</v>
@@ -2951,7 +2979,7 @@
     </row>
     <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>2</v>
@@ -2982,7 +3010,7 @@
     </row>
     <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>2</v>
@@ -3779,7 +3807,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3798,7 +3826,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -3815,13 +3843,13 @@
     </row>
     <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>20</v>
@@ -3831,106 +3859,46 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2000000</v>
-      </c>
-      <c r="E3" s="7">
-        <v>1.0000000000000001E-5</v>
-      </c>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="7">
-        <v>500000</v>
-      </c>
-      <c r="E4" s="7">
-        <v>1.5E-5</v>
-      </c>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="7">
-        <v>300000</v>
-      </c>
-      <c r="E5" s="7">
-        <v>2.0000000000000002E-5</v>
-      </c>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="7">
-        <v>150000</v>
-      </c>
-      <c r="E6" s="7">
-        <v>3.0000000000000001E-5</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="7">
-        <v>50000</v>
-      </c>
-      <c r="E7" s="7">
-        <v>2.5000000000000001E-5</v>
-      </c>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="7">
-        <v>20000</v>
-      </c>
-      <c r="E8" s="7">
-        <v>3.0000000000000001E-5</v>
-      </c>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
@@ -4258,9 +4226,9 @@
   </sheetPr>
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3:D8"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4278,7 +4246,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -4292,7 +4260,7 @@
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
@@ -4306,7 +4274,7 @@
     </row>
     <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>2</v>
@@ -4320,7 +4288,7 @@
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
@@ -4334,7 +4302,7 @@
     </row>
     <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
@@ -4348,7 +4316,7 @@
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>2</v>
@@ -4362,7 +4330,7 @@
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>2</v>
@@ -4376,7 +4344,7 @@
     </row>
     <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>2</v>
@@ -4672,7 +4640,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4681,7 +4649,7 @@
     <col min="2" max="3" width="34.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" style="9" customWidth="1"/>
     <col min="5" max="5" width="28.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="9" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" style="9" customWidth="1"/>
     <col min="8" max="8" width="23.85546875" style="9" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" style="9" customWidth="1"/>
@@ -4691,7 +4659,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>23</v>
@@ -4711,87 +4679,183 @@
     </row>
     <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="11">
+        <v>69448.289999999994</v>
+      </c>
+      <c r="E3" s="12">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="11">
+        <v>100694.46</v>
+      </c>
+      <c r="E4" s="12">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="11">
+        <v>11984.17</v>
+      </c>
+      <c r="E5" s="12">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="A6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="11">
+        <v>3307.02</v>
+      </c>
+      <c r="E6" s="12">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="11">
+        <v>3781.28</v>
+      </c>
+      <c r="E7" s="12">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="A8" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="11">
+        <v>26066.12</v>
+      </c>
+      <c r="E8" s="12">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="A9" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="11">
+        <v>19730</v>
+      </c>
+      <c r="E9" s="12">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="A10" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="11">
+        <v>219279.81</v>
+      </c>
+      <c r="E10" s="12">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
@@ -5132,6 +5196,7 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5142,7 +5207,7 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
@@ -5165,13 +5230,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>5</v>
@@ -5194,31 +5259,31 @@
     </row>
     <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>